<commit_message>
added an input field
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\copy\mehul\Coding\python\google_finance_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAE6FED-D2DC-4719-814F-6175E7750FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC74AB3-103F-4778-A4F4-88D4D5432E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Improve error handling and update README with new instructions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\copy\mehul\Coding\python\google_finance_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC74AB3-103F-4778-A4F4-88D4D5432E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B515D8-3D96-433F-8A92-963E4BC497AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Stock name</t>
   </si>
@@ -42,88 +42,121 @@
     <t>Sell price</t>
   </si>
   <si>
-    <t>TATA MOTORS LIMITED</t>
-  </si>
-  <si>
-    <t>INE155A01022</t>
-  </si>
-  <si>
-    <t>25-02-2022</t>
-  </si>
-  <si>
-    <t>16-05-2024</t>
-  </si>
-  <si>
     <t>Buy date(DD-MM-YYYY)</t>
   </si>
   <si>
     <t>Sell date(DD-MM-YYYY)</t>
   </si>
   <si>
-    <t>COAL INDIA LTD</t>
-  </si>
-  <si>
-    <t>INE522F01014</t>
-  </si>
-  <si>
-    <t>03-03-2022</t>
-  </si>
-  <si>
-    <t>15-03-2024</t>
-  </si>
-  <si>
-    <t>DLF LIMITED</t>
-  </si>
-  <si>
-    <t>INE271C01023</t>
-  </si>
-  <si>
-    <t>07-04-2022</t>
-  </si>
-  <si>
-    <t>INDIAN RAILWAY FIN CORP L</t>
-  </si>
-  <si>
-    <t>INE053F01010</t>
-  </si>
-  <si>
-    <t>08-08-2023</t>
-  </si>
-  <si>
-    <t>13-03-2024</t>
-  </si>
-  <si>
-    <t>OIL AND NATURAL GAS CORP.</t>
-  </si>
-  <si>
-    <t>INE213A01029</t>
-  </si>
-  <si>
-    <t>05-09-2023</t>
-  </si>
-  <si>
-    <t>04-06-2024</t>
-  </si>
-  <si>
     <t>Do not change the format</t>
   </si>
   <si>
-    <t>ASHOK LEYLAND LTD</t>
-  </si>
-  <si>
-    <t>INE208A01029</t>
-  </si>
-  <si>
-    <t>07-06-2024</t>
-  </si>
-  <si>
-    <t>CROMPT GREA CON ELEC LTD</t>
-  </si>
-  <si>
-    <t>INE299U01018</t>
-  </si>
-  <si>
     <t>First enter the realized trades then enter the unrealized trades</t>
+  </si>
+  <si>
+    <t>KITEX GARMENTS LTD</t>
+  </si>
+  <si>
+    <t>INE602G01020</t>
+  </si>
+  <si>
+    <t>13-09-2024</t>
+  </si>
+  <si>
+    <t>19-09-2024</t>
+  </si>
+  <si>
+    <t>MUNJAL AUTO IND. LTD.</t>
+  </si>
+  <si>
+    <t>INE672B01032</t>
+  </si>
+  <si>
+    <t>16-09-2024</t>
+  </si>
+  <si>
+    <t>GEOJIT FINANCIAL SER L</t>
+  </si>
+  <si>
+    <t>INE007B01023</t>
+  </si>
+  <si>
+    <t>17-09-2024</t>
+  </si>
+  <si>
+    <t>ALPA LABORATORIES LTD</t>
+  </si>
+  <si>
+    <t>INE385I01010</t>
+  </si>
+  <si>
+    <t>ALLIED DIGITAL SERV. LTD</t>
+  </si>
+  <si>
+    <t>INE102I01027</t>
+  </si>
+  <si>
+    <t>RANE ENG VALVE LTD</t>
+  </si>
+  <si>
+    <t>INE222J01013</t>
+  </si>
+  <si>
+    <t>SMS PHARMACEUTICALS LTD.</t>
+  </si>
+  <si>
+    <t>INE812G01025</t>
+  </si>
+  <si>
+    <t>INDRAPRASTHA MEDICAL CORP</t>
+  </si>
+  <si>
+    <t>INE681B01017</t>
+  </si>
+  <si>
+    <t>TEMBO GLOBAL IND LTD</t>
+  </si>
+  <si>
+    <t>INE869Y01010</t>
+  </si>
+  <si>
+    <t>KOPRAN LTD</t>
+  </si>
+  <si>
+    <t>INE082A01010</t>
+  </si>
+  <si>
+    <t>SUPRIYA LIFESCIENCE LTD</t>
+  </si>
+  <si>
+    <t>INE07RO01027</t>
+  </si>
+  <si>
+    <t>IIFL SECURITIES LIMITED</t>
+  </si>
+  <si>
+    <t>INE489L01022</t>
+  </si>
+  <si>
+    <t>BHAGERIA INDUSTRIES LTD</t>
+  </si>
+  <si>
+    <t>INE354C01027</t>
+  </si>
+  <si>
+    <t>18-09-2024</t>
+  </si>
+  <si>
+    <t>WANBURY LIMITED</t>
+  </si>
+  <si>
+    <t>INE107F01022</t>
+  </si>
+  <si>
+    <t>EVEREST KANTO CYLINDERLTD</t>
+  </si>
+  <si>
+    <t>INE184H01027</t>
   </si>
 </sst>
 </file>
@@ -456,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,12 +508,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -494,13 +527,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>4</v>
@@ -510,185 +543,367 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>458</v>
+        <v>508.4</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G4">
-        <v>941.65</v>
+        <v>464.4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>132</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>189.6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
       <c r="G5">
-        <v>401.65</v>
+        <v>119.4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
       <c r="E6">
-        <v>401.95</v>
+        <v>520</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>813.35</v>
+        <v>464.4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7">
-        <v>49.95</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G7">
-        <v>132.5</v>
+        <v>153.51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E8">
-        <v>184.55</v>
+        <v>123.5</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G8">
-        <v>257.5</v>
+        <v>112.71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E9">
-        <v>225.7</v>
+        <v>307.75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>276.75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E10">
-        <v>225.7</v>
+        <v>528.85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>464.4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>404</v>
+        <v>554.79999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>371.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>479.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>351.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>321.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>270.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="E12">
-        <v>404</v>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>329.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>